<commit_message>
Added Fuction to export the file. Starting with the missing values functionalities
</commit_message>
<xml_diff>
--- a/Test.xlsx
+++ b/Test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Siddhaant Pahuja\codes\dataProcessingTool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E0081B7-B31E-46EF-9412-1A371D545019}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24B19433-F8AB-4B17-A1DD-59FB57DCB6BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2160" yWindow="2160" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
   <si>
     <t>Id</t>
   </si>
@@ -51,9 +51,6 @@
     <t>Shelby</t>
   </si>
   <si>
-    <t>Black</t>
-  </si>
-  <si>
     <t>Tia</t>
   </si>
   <si>
@@ -91,6 +88,15 @@
   </si>
   <si>
     <t>Date</t>
+  </si>
+  <si>
+    <t>Bro</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -409,10 +415,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -420,7 +426,7 @@
     <col min="5" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -434,10 +440,13 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -453,8 +462,11 @@
       <c r="E2" s="1">
         <v>45028</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -470,8 +482,11 @@
       <c r="E3" s="1">
         <v>44693</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -484,19 +499,20 @@
       <c r="D4">
         <v>45</v>
       </c>
-      <c r="E4" s="1">
-        <v>44359</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E4" s="1"/>
+      <c r="F4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
         <v>13</v>
-      </c>
-      <c r="C5" t="s">
-        <v>14</v>
       </c>
       <c r="D5">
         <v>33</v>
@@ -504,8 +520,11 @@
       <c r="E5" s="1">
         <v>44024</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -513,7 +532,7 @@
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D6">
         <v>56</v>
@@ -521,16 +540,16 @@
       <c r="E6" s="1">
         <v>43689</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
-        <v>8</v>
-      </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D7">
         <v>43</v>
@@ -538,33 +557,36 @@
       <c r="E7" s="1">
         <v>43355</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8">
-        <v>54</v>
+        <v>16</v>
       </c>
       <c r="E8" s="1">
         <v>43020</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D9">
         <v>33</v>
@@ -573,38 +595,42 @@
         <v>42686</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D10">
         <v>27</v>
       </c>
-      <c r="E10" s="1">
-        <v>42350</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E10" s="1"/>
+      <c r="F10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D11">
         <v>34</v>
       </c>
       <c r="E11" s="1">
         <v>42016</v>
+      </c>
+      <c r="F11" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>